<commit_message>
update data in excell data file
</commit_message>
<xml_diff>
--- a/FoodAR.xlsx
+++ b/FoodAR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/448db3c2dce337ca/Desktop/AR-FoodFinder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itayg\OneDrive\Desktop\AR-FoodFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84458CC7-88F0-48BD-92B8-5681AACF52E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8B7A78-7B8E-4C1D-B5BC-BD1B38AA8BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{DA96FEAB-205F-4F25-B9ED-B68EE0B69310}"/>
   </bookViews>

</xml_diff>

<commit_message>
able to sync data properly. learned that MUST RERUN NPM BUILD START AND USE DATA FROM my-app/public folder
</commit_message>
<xml_diff>
--- a/FoodAR.xlsx
+++ b/FoodAR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itayg\OneDrive\Desktop\AR-FoodFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8B7A78-7B8E-4C1D-B5BC-BD1B38AA8BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84458CC7-88F0-48BD-92B8-5681AACF52E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{DA96FEAB-205F-4F25-B9ED-B68EE0B69310}"/>
   </bookViews>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B187622D-BC7B-4C02-9F26-3594D4840DF8}">
   <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="H133" sqref="H133"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>